<commit_message>
✨I can do it!
</commit_message>
<xml_diff>
--- a/许愿墙.xlsx
+++ b/许愿墙.xlsx
@@ -1,86 +1,288 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dannike/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F99DB62-C54B-5247-A80D-A1B4F1C822C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcMode="auto"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">  </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="64">
+  <si>
+    <t>你想找什么样的工作？</t>
+  </si>
+  <si>
+    <t>现在的状态是怎样的？</t>
+  </si>
+  <si>
+    <t>AI攻城狮</t>
+  </si>
+  <si>
+    <t>已找到！</t>
+  </si>
+  <si>
+    <t>Java+AI</t>
+  </si>
+  <si>
+    <t>在找</t>
+  </si>
+  <si>
+    <t>AI agent开发</t>
+  </si>
+  <si>
+    <t>Java实习</t>
+  </si>
+  <si>
+    <t>还没开始找</t>
+  </si>
+  <si>
+    <t>系统架构师</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>前端攻城狮</t>
+  </si>
+  <si>
+    <t>AI+游戏开发</t>
+  </si>
+  <si>
+    <t>C++实习</t>
+  </si>
+  <si>
+    <t>后端开发</t>
+  </si>
+  <si>
+    <t>正确的路上</t>
+  </si>
+  <si>
+    <t>Java后端开发</t>
+  </si>
+  <si>
+    <t>在找实习的路上</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>找到了，但是通勤太远想跳槽</t>
+  </si>
+  <si>
+    <t>Frontend leader</t>
+  </si>
+  <si>
+    <t>找到了，但是没有work life balance</t>
+  </si>
+  <si>
+    <t>找到了，不满意</t>
+  </si>
+  <si>
+    <t>Java开发</t>
+  </si>
+  <si>
+    <t>再找</t>
+  </si>
+  <si>
+    <t>前端工程师</t>
+  </si>
+  <si>
+    <t>java开发</t>
+  </si>
+  <si>
+    <t>AI+前端工程师</t>
+  </si>
+  <si>
+    <t>C++开发</t>
+  </si>
+  <si>
+    <t>Go后端开发</t>
+  </si>
+  <si>
+    <t>AI+后端工程师</t>
+  </si>
+  <si>
+    <t>linux运维</t>
+  </si>
+  <si>
+    <t>AI+嵌入式</t>
+  </si>
+  <si>
+    <t>财务主管</t>
+  </si>
+  <si>
+    <t>在学习的路上</t>
+  </si>
+  <si>
+    <t>去年7月用这个项目找到了第一份工作，现在再次回来，希望跳槽找一份AI售前的工作</t>
+  </si>
+  <si>
+    <t>准备跳槽</t>
+  </si>
+  <si>
+    <t>Java开发，有完善的晋升制度</t>
+  </si>
+  <si>
+    <t>前端开发</t>
+  </si>
+  <si>
+    <t>找到了，兄弟们加油。对于前端这块简历一定要吹牛逼写好，
+面试前真的要背好八股和场景，或者找不想去的公司练练手，准备好了之后再冲刺</t>
+  </si>
+  <si>
+    <t>正在找</t>
+  </si>
+  <si>
+    <t>C#开发</t>
+  </si>
+  <si>
+    <t>dotnet开发，base 成都</t>
+  </si>
+  <si>
+    <t>JAVA开发，base太原</t>
+  </si>
+  <si>
+    <t>前端开发，base上海</t>
+  </si>
+  <si>
+    <t>测试开发</t>
+  </si>
+  <si>
+    <t>运维开发</t>
+  </si>
+  <si>
+    <t>找到了，要去当牛马了，后续准备做独立开发</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 渗透测试工程师</t>
+  </si>
+  <si>
+    <t>应届在找</t>
+  </si>
+  <si>
+    <t>IT审计/数据分析/财务BP</t>
+  </si>
+  <si>
+    <t>AI应用开发</t>
+  </si>
+  <si>
+    <t>设计师</t>
+  </si>
+  <si>
+    <t>Java开发/海外仓销售</t>
+  </si>
+  <si>
+    <t>ai产品</t>
+  </si>
+  <si>
+    <t>数据开发+ai</t>
+  </si>
+  <si>
+    <t>失业了在找</t>
+  </si>
+  <si>
+    <t>AI+JAVA</t>
+  </si>
+  <si>
+    <t>大专，前端工程师，空窗创业，gap一年半😁，找了内推看看机会
+保持学习，看下金九银十有没机会了</t>
+  </si>
+  <si>
+    <t>AI产品</t>
+  </si>
+  <si>
+    <t>Java秋招</t>
+  </si>
+  <si>
+    <t>目前实习，在改简历背八股准备秋招！！！</t>
+  </si>
+  <si>
+    <t>AIGC相关后端或全栈/量化交易员</t>
+  </si>
+  <si>
+    <t>在找，之前上过大厂班，不适应，后续我想做独立开发</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF34C724"/>
-        <bgColor/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -162,38 +364,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDEE0E3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDEE0E3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDEE0E3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDEE0E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -206,7 +429,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -501,28 +724,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="false" summaryRight="false"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="74"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="54"/>
+    <col min="1" max="1" width="74" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="str">
-        <v>你想找什么样的工作？</v>
-      </c>
-      <c r="B1" s="6" t="str">
-        <v>现在的状态是怎样的？</v>
+    <row r="1" spans="1:20">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -543,12 +766,12 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="str">
-        <v>AI攻城狮</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <v>已找到！</v>
+    <row r="2" spans="1:20">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -569,12 +792,12 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="str">
-        <v>Java+AI</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <v>在找</v>
+    <row r="3" spans="1:20">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -595,12 +818,12 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="str">
-        <v>AI agent开发</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <v>在找</v>
+    <row r="4" spans="1:20">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -621,12 +844,12 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="str">
-        <v>Java实习</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <v>还没开始找</v>
+    <row r="5" spans="1:20">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -647,12 +870,12 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="str">
-        <v>系统架构师</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <v>在找</v>
+    <row r="6" spans="1:20">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -673,12 +896,12 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="str">
-        <v>Go</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <v>在找</v>
+    <row r="7" spans="1:20">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -699,12 +922,12 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="str">
-        <v>前端攻城狮</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <v>在找</v>
+    <row r="8" spans="1:20">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -725,12 +948,12 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="str">
-        <v>AI+游戏开发</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <v>在找</v>
+    <row r="9" spans="1:20">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -751,12 +974,12 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="str">
-        <v>C++实习</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <v>在找</v>
+    <row r="10" spans="1:20">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -777,12 +1000,12 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="str">
-        <v>后端开发</v>
-      </c>
-      <c r="B11" s="2" t="str">
-        <v>正确的路上</v>
+    <row r="11" spans="1:20">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -803,12 +1026,12 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="str">
-        <v>Java后端开发</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <v>在找实习的路上</v>
+    <row r="12" spans="1:20">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -829,12 +1052,12 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="str">
-        <v>Java</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <v>找到了，但是通勤太远想跳槽</v>
+    <row r="13" spans="1:20">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -855,12 +1078,12 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="str">
-        <v>Frontend leader</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <v>找到了，但是没有work life balance</v>
+    <row r="14" spans="1:20">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -881,12 +1104,12 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="str">
-        <v>Java</v>
-      </c>
-      <c r="B15" s="2" t="str">
-        <v>找到了，不满意</v>
+    <row r="15" spans="1:20">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -907,12 +1130,12 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="str">
-        <v>Java开发</v>
-      </c>
-      <c r="B16" s="2" t="str">
-        <v>再找</v>
+    <row r="16" spans="1:20">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -933,12 +1156,12 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="str">
-        <v>前端工程师</v>
-      </c>
-      <c r="B17" s="2" t="str">
-        <v>在找</v>
+    <row r="17" spans="1:20">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -959,12 +1182,12 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="str">
-        <v>java开发</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <v>在找</v>
+    <row r="18" spans="1:20">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -985,12 +1208,12 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="str">
-        <v>AI+前端工程师</v>
-      </c>
-      <c r="B19" s="2" t="str">
-        <v>还没开始找</v>
+    <row r="19" spans="1:20">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1011,12 +1234,12 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="str">
-        <v>C++开发</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <v>在找</v>
+    <row r="20" spans="1:20">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1037,12 +1260,12 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="str">
-        <v>Go</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <v>在找</v>
+    <row r="21" spans="1:20">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1063,12 +1286,12 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="str">
-        <v>Go后端开发</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <v>在找</v>
+    <row r="22" spans="1:20">
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1089,12 +1312,12 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="str">
-        <v>AI+后端工程师</v>
-      </c>
-      <c r="B23" s="2" t="str">
-        <v>还没开始找</v>
+    <row r="23" spans="1:20">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1115,12 +1338,12 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="str">
-        <v>linux运维</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <v>在找</v>
+    <row r="24" spans="1:20">
+      <c r="A24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1141,12 +1364,12 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="str">
-        <v>前端工程师</v>
-      </c>
-      <c r="B25" s="2" t="str">
-        <v>在找</v>
+    <row r="25" spans="1:20">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1167,12 +1390,12 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26">
-      <c r="A26" s="2" t="str">
-        <v>前端工程师</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <v>还没开始找</v>
+    <row r="26" spans="1:20">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1193,12 +1416,12 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="str">
-        <v>java开发</v>
-      </c>
-      <c r="B27" s="2" t="str">
-        <v>在找</v>
+    <row r="27" spans="1:20">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1219,12 +1442,12 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="str">
-        <v>AI+嵌入式</v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <v>再找</v>
+    <row r="28" spans="1:20">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1245,12 +1468,12 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="str">
-        <v>财务主管</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <v>在找</v>
+    <row r="29" spans="1:20">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1271,12 +1494,12 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="str">
-        <v>后端开发</v>
-      </c>
-      <c r="B30" s="2" t="str">
-        <v>在学习的路上</v>
+    <row r="30" spans="1:20">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1297,12 +1520,12 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="str">
-        <v>去年7月用这个项目找到了第一份工作，现在再次回来，希望跳槽找一份AI售前的工作</v>
-      </c>
-      <c r="B31" s="2" t="str">
-        <v>在找</v>
+    <row r="31" spans="1:20">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1323,12 +1546,12 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="str">
-        <v>前端工程师</v>
-      </c>
-      <c r="B32" s="2" t="str">
-        <v>在找</v>
+    <row r="32" spans="1:20">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1349,12 +1572,12 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="str">
-        <v>Java开发</v>
-      </c>
-      <c r="B33" s="2" t="str">
-        <v>准备跳槽</v>
+    <row r="33" spans="1:20">
+      <c r="A33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1375,12 +1598,12 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="str">
-        <v>Java开发，有完善的晋升制度</v>
-      </c>
-      <c r="B34" s="2" t="str">
-        <v>准备跳槽</v>
+    <row r="34" spans="1:20">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1401,13 +1624,12 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="str">
-        <v>前端开发</v>
-      </c>
-      <c r="B35" s="2" t="str">
-        <v>找到了，兄弟们加油。对于前端这块简历一定要吹牛逼写好，
-面试前真的要背好八股和场景，或者找不想去的公司练练手，准备好了之后再冲刺</v>
+    <row r="35" spans="1:20">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1428,12 +1650,12 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="str">
-        <v>java开发</v>
-      </c>
-      <c r="B36" s="2" t="str">
-        <v>在找</v>
+    <row r="36" spans="1:20">
+      <c r="A36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1454,12 +1676,12 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="str">
-        <v>Java开发</v>
-      </c>
-      <c r="B37" s="2" t="str">
-        <v>正在找</v>
+    <row r="37" spans="1:20">
+      <c r="A37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1480,12 +1702,12 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="str">
-        <v>Java+AI</v>
-      </c>
-      <c r="B38" s="2" t="str">
-        <v>在找</v>
+    <row r="38" spans="1:20">
+      <c r="A38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1506,12 +1728,12 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39">
-      <c r="A39" s="4" t="str">
-        <v>AI+后端工程师</v>
-      </c>
-      <c r="B39" s="2" t="str">
-        <v>在找</v>
+    <row r="39" spans="1:20">
+      <c r="A39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1532,12 +1754,12 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="str">
-        <v>java开发</v>
-      </c>
-      <c r="B40" s="2" t="str">
-        <v>在找</v>
+    <row r="40" spans="1:20">
+      <c r="A40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1558,12 +1780,12 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="str">
-        <v>C#开发</v>
-      </c>
-      <c r="B41" s="2" t="str">
-        <v>在找</v>
+    <row r="41" spans="1:20">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1584,12 +1806,12 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="str">
-        <v>dotnet开发，base 成都</v>
-      </c>
-      <c r="B42" s="2" t="str">
-        <v>准备跳槽</v>
+    <row r="42" spans="1:20">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1610,12 +1832,12 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="str">
-        <v>JAVA开发，base太原</v>
-      </c>
-      <c r="B43" s="2" t="str">
-        <v>在找</v>
+    <row r="43" spans="1:20">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1636,12 +1858,12 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="str">
-        <v>Java开发</v>
-      </c>
-      <c r="B44" s="2" t="str">
-        <v>准备跳槽</v>
+    <row r="44" spans="1:20">
+      <c r="A44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1662,12 +1884,12 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="str">
-        <v>前端开发，base上海</v>
-      </c>
-      <c r="B45" s="2" t="str">
-        <v>在找</v>
+    <row r="45" spans="1:20">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1688,12 +1910,12 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="str">
-        <v>测试开发</v>
-      </c>
-      <c r="B46" s="2" t="str">
-        <v>在找</v>
+    <row r="46" spans="1:20">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1714,12 +1936,12 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47">
-      <c r="A47" s="5" t="str">
-        <v>运维开发</v>
-      </c>
-      <c r="B47" s="2" t="str">
-        <v>找到了，要去当牛马了，后续准备做独立开发</v>
+    <row r="47" spans="1:20">
+      <c r="A47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1740,12 +1962,12 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="str" xml:space="preserve">
-        <v> 渗透测试工程师</v>
-      </c>
-      <c r="B48" s="2" t="str">
-        <v>应届在找</v>
+    <row r="48" spans="1:20">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1766,12 +1988,12 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="str">
-        <v>IT审计/数据分析/财务BP</v>
-      </c>
-      <c r="B49" s="2" t="str">
-        <v>准备跳槽</v>
+    <row r="49" spans="1:20">
+      <c r="A49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1792,12 +2014,12 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="str">
-        <v>AI应用开发</v>
-      </c>
-      <c r="B50" s="2" t="str">
-        <v>在找</v>
+    <row r="50" spans="1:20">
+      <c r="A50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1818,12 +2040,12 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="str">
-        <v>设计师</v>
-      </c>
-      <c r="B51" s="2" t="str">
-        <v>在找</v>
+    <row r="51" spans="1:20">
+      <c r="A51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1844,12 +2066,12 @@
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="str">
-        <v>运维开发</v>
-      </c>
-      <c r="B52" s="2" t="str">
-        <v>在找</v>
+    <row r="52" spans="1:20">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1870,12 +2092,12 @@
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="str">
-        <v>Java开发</v>
-      </c>
-      <c r="B53" s="2" t="str">
-        <v>在找</v>
+    <row r="53" spans="1:20">
+      <c r="A53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1896,12 +2118,12 @@
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="str">
-        <v>Java开发/海外仓销售</v>
-      </c>
-      <c r="B54" s="2" t="str">
-        <v>在找</v>
+    <row r="54" spans="1:20">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1922,12 +2144,12 @@
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="str">
-        <v>ai产品</v>
-      </c>
-      <c r="B55" s="2" t="str">
-        <v>在找</v>
+    <row r="55" spans="1:20">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1948,12 +2170,12 @@
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="str">
-        <v>ai产品</v>
-      </c>
-      <c r="B56" s="2" t="str">
-        <v>在找</v>
+    <row r="56" spans="1:20">
+      <c r="A56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1974,12 +2196,12 @@
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="str">
-        <v>数据开发+ai</v>
-      </c>
-      <c r="B57" s="2" t="str">
-        <v>失业了在找</v>
+    <row r="57" spans="1:20">
+      <c r="A57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2000,12 +2222,12 @@
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="str">
-        <v>AI+JAVA</v>
-      </c>
-      <c r="B58" s="2" t="str">
-        <v>在找</v>
+    <row r="58" spans="1:20">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2026,12 +2248,12 @@
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="str">
-        <v>Java实习</v>
-      </c>
-      <c r="B59" s="2" t="str">
-        <v>在找</v>
+    <row r="59" spans="1:20">
+      <c r="A59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2052,13 +2274,12 @@
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="str">
-        <v>前端工程师</v>
-      </c>
-      <c r="B60" s="2" t="str">
-        <v>大专，前端工程师，空窗创业，gap一年半😁，找了内推看看机会
-保持学习，看下金九银十有没机会了</v>
+    <row r="60" spans="1:20">
+      <c r="A60" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2079,12 +2300,12 @@
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="str">
-        <v>AI产品</v>
-      </c>
-      <c r="B61" s="2" t="str">
-        <v>在找</v>
+    <row r="61" spans="1:20">
+      <c r="A61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2105,12 +2326,12 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="str">
-        <v>Java秋招</v>
-      </c>
-      <c r="B62" s="2" t="str">
-        <v>目前实习，在改简历背八股准备秋招！！！</v>
+    <row r="62" spans="1:20">
+      <c r="A62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2131,9 +2352,13 @@
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
     </row>
-    <row r="63">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
+    <row r="63" spans="1:20">
+      <c r="A63" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2153,8 +2378,7 @@
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
     </row>
-    <row r="64">
-      <c r="A64" s="2"/>
+    <row r="64" spans="1:20">
       <c r="B64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2175,7 +2399,7 @@
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:20">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="1"/>
@@ -2197,7 +2421,7 @@
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:20">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="1"/>
@@ -2219,7 +2443,7 @@
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:20">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="1"/>
@@ -2241,7 +2465,7 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:20">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="1"/>
@@ -2263,7 +2487,7 @@
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:20">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="1"/>
@@ -2285,7 +2509,7 @@
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:20">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="1"/>
@@ -2307,7 +2531,7 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:20">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="1"/>
@@ -2329,7 +2553,7 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:20">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
@@ -2351,7 +2575,7 @@
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:20">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="1"/>
@@ -2373,7 +2597,7 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:20">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="1"/>
@@ -2395,7 +2619,7 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:20">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="1"/>
@@ -2417,7 +2641,7 @@
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:20">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="1"/>
@@ -2439,7 +2663,7 @@
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:20">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="1"/>
@@ -2461,7 +2685,7 @@
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:20">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="1"/>
@@ -2483,7 +2707,7 @@
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:20">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="1"/>
@@ -2505,7 +2729,7 @@
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:20">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="1"/>
@@ -2527,7 +2751,7 @@
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:20">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="1"/>
@@ -2549,7 +2773,7 @@
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:20">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="1"/>
@@ -2571,7 +2795,7 @@
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:20">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="1"/>
@@ -2593,7 +2817,7 @@
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:20">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
@@ -2615,7 +2839,7 @@
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:20">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
@@ -2637,7 +2861,7 @@
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:20">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
@@ -2659,7 +2883,7 @@
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:20">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="1"/>
@@ -2681,7 +2905,7 @@
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:20">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="1"/>
@@ -2703,7 +2927,7 @@
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:20">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="1"/>
@@ -2725,7 +2949,7 @@
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:20">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="1"/>
@@ -2747,7 +2971,7 @@
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:20">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
@@ -2769,7 +2993,7 @@
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:20">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="1"/>
@@ -2791,7 +3015,7 @@
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:20">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
@@ -2813,7 +3037,7 @@
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:20">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
@@ -2835,7 +3059,7 @@
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:20">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
@@ -2857,7 +3081,7 @@
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:20">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
@@ -2879,7 +3103,7 @@
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:20">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
@@ -2901,7 +3125,7 @@
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:20">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="1"/>
@@ -2923,7 +3147,7 @@
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:20">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="1"/>
@@ -2945,7 +3169,7 @@
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:20">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="1"/>
@@ -2967,7 +3191,7 @@
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:20">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
@@ -2989,7 +3213,7 @@
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:20">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
@@ -3011,7 +3235,7 @@
       <c r="S102" s="1"/>
       <c r="T102" s="1"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:20">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="1"/>
@@ -3033,7 +3257,7 @@
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:20">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="1"/>
@@ -3055,7 +3279,7 @@
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:20">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="1"/>
@@ -3077,7 +3301,7 @@
       <c r="S105" s="1"/>
       <c r="T105" s="1"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:20">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="1"/>
@@ -3099,7 +3323,7 @@
       <c r="S106" s="1"/>
       <c r="T106" s="1"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:20">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="1"/>
@@ -3121,7 +3345,7 @@
       <c r="S107" s="1"/>
       <c r="T107" s="1"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:20">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="1"/>
@@ -3143,7 +3367,7 @@
       <c r="S108" s="1"/>
       <c r="T108" s="1"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:20">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="1"/>
@@ -3165,7 +3389,7 @@
       <c r="S109" s="1"/>
       <c r="T109" s="1"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:20">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="1"/>
@@ -3187,7 +3411,7 @@
       <c r="S110" s="1"/>
       <c r="T110" s="1"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:20">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="1"/>
@@ -3209,7 +3433,7 @@
       <c r="S111" s="1"/>
       <c r="T111" s="1"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:20">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
@@ -3231,7 +3455,7 @@
       <c r="S112" s="1"/>
       <c r="T112" s="1"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:20">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="1"/>
@@ -3253,7 +3477,7 @@
       <c r="S113" s="1"/>
       <c r="T113" s="1"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:20">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="1"/>
@@ -3275,7 +3499,7 @@
       <c r="S114" s="1"/>
       <c r="T114" s="1"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:20">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="1"/>
@@ -3297,7 +3521,7 @@
       <c r="S115" s="1"/>
       <c r="T115" s="1"/>
     </row>
-    <row r="116">
+    <row r="116" spans="1:20">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="1"/>
@@ -3319,7 +3543,7 @@
       <c r="S116" s="1"/>
       <c r="T116" s="1"/>
     </row>
-    <row r="117">
+    <row r="117" spans="1:20">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="1"/>
@@ -3341,7 +3565,7 @@
       <c r="S117" s="1"/>
       <c r="T117" s="1"/>
     </row>
-    <row r="118">
+    <row r="118" spans="1:20">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="1"/>
@@ -3363,7 +3587,7 @@
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
     </row>
-    <row r="119">
+    <row r="119" spans="1:20">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="1"/>
@@ -3385,7 +3609,7 @@
       <c r="S119" s="1"/>
       <c r="T119" s="1"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:20">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="1"/>
@@ -3407,7 +3631,7 @@
       <c r="S120" s="1"/>
       <c r="T120" s="1"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:20">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="1"/>
@@ -3429,7 +3653,7 @@
       <c r="S121" s="1"/>
       <c r="T121" s="1"/>
     </row>
-    <row r="122">
+    <row r="122" spans="1:20">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="1"/>
@@ -3451,7 +3675,7 @@
       <c r="S122" s="1"/>
       <c r="T122" s="1"/>
     </row>
-    <row r="123">
+    <row r="123" spans="1:20">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="1"/>
@@ -3473,7 +3697,7 @@
       <c r="S123" s="1"/>
       <c r="T123" s="1"/>
     </row>
-    <row r="124">
+    <row r="124" spans="1:20">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
@@ -3495,7 +3719,7 @@
       <c r="S124" s="1"/>
       <c r="T124" s="1"/>
     </row>
-    <row r="125">
+    <row r="125" spans="1:20">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
@@ -3517,7 +3741,7 @@
       <c r="S125" s="1"/>
       <c r="T125" s="1"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:20">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
@@ -3539,7 +3763,7 @@
       <c r="S126" s="1"/>
       <c r="T126" s="1"/>
     </row>
-    <row r="127">
+    <row r="127" spans="1:20">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
@@ -3561,7 +3785,7 @@
       <c r="S127" s="1"/>
       <c r="T127" s="1"/>
     </row>
-    <row r="128">
+    <row r="128" spans="1:20">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="1"/>
@@ -3583,7 +3807,7 @@
       <c r="S128" s="1"/>
       <c r="T128" s="1"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:20">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="1"/>
@@ -3605,7 +3829,7 @@
       <c r="S129" s="1"/>
       <c r="T129" s="1"/>
     </row>
-    <row r="130">
+    <row r="130" spans="1:20">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="1"/>
@@ -3627,7 +3851,7 @@
       <c r="S130" s="1"/>
       <c r="T130" s="1"/>
     </row>
-    <row r="131">
+    <row r="131" spans="1:20">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="1"/>
@@ -3649,7 +3873,7 @@
       <c r="S131" s="1"/>
       <c r="T131" s="1"/>
     </row>
-    <row r="132">
+    <row r="132" spans="1:20">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="1"/>
@@ -3671,7 +3895,7 @@
       <c r="S132" s="1"/>
       <c r="T132" s="1"/>
     </row>
-    <row r="133">
+    <row r="133" spans="1:20">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="1"/>
@@ -3693,7 +3917,7 @@
       <c r="S133" s="1"/>
       <c r="T133" s="1"/>
     </row>
-    <row r="134">
+    <row r="134" spans="1:20">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="1"/>
@@ -3715,7 +3939,7 @@
       <c r="S134" s="1"/>
       <c r="T134" s="1"/>
     </row>
-    <row r="135">
+    <row r="135" spans="1:20">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="1"/>
@@ -3737,7 +3961,7 @@
       <c r="S135" s="1"/>
       <c r="T135" s="1"/>
     </row>
-    <row r="136">
+    <row r="136" spans="1:20">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="1"/>
@@ -3759,7 +3983,7 @@
       <c r="S136" s="1"/>
       <c r="T136" s="1"/>
     </row>
-    <row r="137">
+    <row r="137" spans="1:20">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="1"/>
@@ -3781,7 +4005,7 @@
       <c r="S137" s="1"/>
       <c r="T137" s="1"/>
     </row>
-    <row r="138">
+    <row r="138" spans="1:20">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="1"/>
@@ -3803,7 +4027,7 @@
       <c r="S138" s="1"/>
       <c r="T138" s="1"/>
     </row>
-    <row r="139">
+    <row r="139" spans="1:20">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="1"/>
@@ -3825,7 +4049,7 @@
       <c r="S139" s="1"/>
       <c r="T139" s="1"/>
     </row>
-    <row r="140">
+    <row r="140" spans="1:20">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
@@ -3847,7 +4071,7 @@
       <c r="S140" s="1"/>
       <c r="T140" s="1"/>
     </row>
-    <row r="141">
+    <row r="141" spans="1:20">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="1"/>
@@ -3869,7 +4093,7 @@
       <c r="S141" s="1"/>
       <c r="T141" s="1"/>
     </row>
-    <row r="142">
+    <row r="142" spans="1:20">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="1"/>
@@ -3891,7 +4115,7 @@
       <c r="S142" s="1"/>
       <c r="T142" s="1"/>
     </row>
-    <row r="143">
+    <row r="143" spans="1:20">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="1"/>
@@ -3913,7 +4137,7 @@
       <c r="S143" s="1"/>
       <c r="T143" s="1"/>
     </row>
-    <row r="144">
+    <row r="144" spans="1:20">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="1"/>
@@ -3935,7 +4159,7 @@
       <c r="S144" s="1"/>
       <c r="T144" s="1"/>
     </row>
-    <row r="145">
+    <row r="145" spans="1:20">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="1"/>
@@ -3957,7 +4181,7 @@
       <c r="S145" s="1"/>
       <c r="T145" s="1"/>
     </row>
-    <row r="146">
+    <row r="146" spans="1:20">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="1"/>
@@ -3979,7 +4203,7 @@
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
     </row>
-    <row r="147">
+    <row r="147" spans="1:20">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="1"/>
@@ -4001,7 +4225,7 @@
       <c r="S147" s="1"/>
       <c r="T147" s="1"/>
     </row>
-    <row r="148">
+    <row r="148" spans="1:20">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="1"/>
@@ -4023,7 +4247,7 @@
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
     </row>
-    <row r="149">
+    <row r="149" spans="1:20">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="1"/>
@@ -4045,7 +4269,7 @@
       <c r="S149" s="1"/>
       <c r="T149" s="1"/>
     </row>
-    <row r="150">
+    <row r="150" spans="1:20">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="1"/>
@@ -4067,7 +4291,7 @@
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
     </row>
-    <row r="151">
+    <row r="151" spans="1:20">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="1"/>
@@ -4089,7 +4313,7 @@
       <c r="S151" s="1"/>
       <c r="T151" s="1"/>
     </row>
-    <row r="152">
+    <row r="152" spans="1:20">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="1"/>
@@ -4111,7 +4335,7 @@
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
     </row>
-    <row r="153">
+    <row r="153" spans="1:20">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="1"/>
@@ -4133,7 +4357,7 @@
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
     </row>
-    <row r="154">
+    <row r="154" spans="1:20">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="1"/>
@@ -4155,7 +4379,7 @@
       <c r="S154" s="1"/>
       <c r="T154" s="1"/>
     </row>
-    <row r="155">
+    <row r="155" spans="1:20">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="1"/>
@@ -4177,7 +4401,7 @@
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
     </row>
-    <row r="156">
+    <row r="156" spans="1:20">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="1"/>
@@ -4199,7 +4423,7 @@
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
     </row>
-    <row r="157">
+    <row r="157" spans="1:20">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="1"/>
@@ -4221,7 +4445,7 @@
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
     </row>
-    <row r="158">
+    <row r="158" spans="1:20">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="1"/>
@@ -4243,7 +4467,7 @@
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
     </row>
-    <row r="159">
+    <row r="159" spans="1:20">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="1"/>
@@ -4265,7 +4489,7 @@
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
     </row>
-    <row r="160">
+    <row r="160" spans="1:20">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="1"/>
@@ -4287,7 +4511,7 @@
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
     </row>
-    <row r="161">
+    <row r="161" spans="1:20">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="1"/>
@@ -4309,7 +4533,7 @@
       <c r="S161" s="1"/>
       <c r="T161" s="1"/>
     </row>
-    <row r="162">
+    <row r="162" spans="1:20">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="1"/>
@@ -4331,7 +4555,7 @@
       <c r="S162" s="1"/>
       <c r="T162" s="1"/>
     </row>
-    <row r="163">
+    <row r="163" spans="1:20">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="1"/>
@@ -4353,7 +4577,7 @@
       <c r="S163" s="1"/>
       <c r="T163" s="1"/>
     </row>
-    <row r="164">
+    <row r="164" spans="1:20">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="1"/>
@@ -4375,7 +4599,7 @@
       <c r="S164" s="1"/>
       <c r="T164" s="1"/>
     </row>
-    <row r="165">
+    <row r="165" spans="1:20">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="1"/>
@@ -4397,7 +4621,7 @@
       <c r="S165" s="1"/>
       <c r="T165" s="1"/>
     </row>
-    <row r="166">
+    <row r="166" spans="1:20">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="1"/>
@@ -4419,7 +4643,7 @@
       <c r="S166" s="1"/>
       <c r="T166" s="1"/>
     </row>
-    <row r="167">
+    <row r="167" spans="1:20">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="1"/>
@@ -4441,7 +4665,7 @@
       <c r="S167" s="1"/>
       <c r="T167" s="1"/>
     </row>
-    <row r="168">
+    <row r="168" spans="1:20">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="1"/>
@@ -4463,7 +4687,7 @@
       <c r="S168" s="1"/>
       <c r="T168" s="1"/>
     </row>
-    <row r="169">
+    <row r="169" spans="1:20">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="1"/>
@@ -4485,7 +4709,7 @@
       <c r="S169" s="1"/>
       <c r="T169" s="1"/>
     </row>
-    <row r="170">
+    <row r="170" spans="1:20">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="1"/>
@@ -4507,7 +4731,7 @@
       <c r="S170" s="1"/>
       <c r="T170" s="1"/>
     </row>
-    <row r="171">
+    <row r="171" spans="1:20">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="1"/>
@@ -4529,7 +4753,7 @@
       <c r="S171" s="1"/>
       <c r="T171" s="1"/>
     </row>
-    <row r="172">
+    <row r="172" spans="1:20">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="1"/>
@@ -4551,7 +4775,7 @@
       <c r="S172" s="1"/>
       <c r="T172" s="1"/>
     </row>
-    <row r="173">
+    <row r="173" spans="1:20">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="1"/>
@@ -4573,7 +4797,7 @@
       <c r="S173" s="1"/>
       <c r="T173" s="1"/>
     </row>
-    <row r="174">
+    <row r="174" spans="1:20">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="1"/>
@@ -4595,7 +4819,7 @@
       <c r="S174" s="1"/>
       <c r="T174" s="1"/>
     </row>
-    <row r="175">
+    <row r="175" spans="1:20">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="1"/>
@@ -4617,7 +4841,7 @@
       <c r="S175" s="1"/>
       <c r="T175" s="1"/>
     </row>
-    <row r="176">
+    <row r="176" spans="1:20">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="1"/>
@@ -4639,7 +4863,7 @@
       <c r="S176" s="1"/>
       <c r="T176" s="1"/>
     </row>
-    <row r="177">
+    <row r="177" spans="1:20">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="1"/>
@@ -4661,7 +4885,7 @@
       <c r="S177" s="1"/>
       <c r="T177" s="1"/>
     </row>
-    <row r="178">
+    <row r="178" spans="1:20">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="1"/>
@@ -4683,7 +4907,7 @@
       <c r="S178" s="1"/>
       <c r="T178" s="1"/>
     </row>
-    <row r="179">
+    <row r="179" spans="1:20">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="1"/>
@@ -4705,7 +4929,7 @@
       <c r="S179" s="1"/>
       <c r="T179" s="1"/>
     </row>
-    <row r="180">
+    <row r="180" spans="1:20">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="1"/>
@@ -4727,7 +4951,7 @@
       <c r="S180" s="1"/>
       <c r="T180" s="1"/>
     </row>
-    <row r="181">
+    <row r="181" spans="1:20">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="1"/>
@@ -4749,7 +4973,7 @@
       <c r="S181" s="1"/>
       <c r="T181" s="1"/>
     </row>
-    <row r="182">
+    <row r="182" spans="1:20">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="1"/>
@@ -4771,7 +4995,7 @@
       <c r="S182" s="1"/>
       <c r="T182" s="1"/>
     </row>
-    <row r="183">
+    <row r="183" spans="1:20">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="1"/>
@@ -4793,7 +5017,7 @@
       <c r="S183" s="1"/>
       <c r="T183" s="1"/>
     </row>
-    <row r="184">
+    <row r="184" spans="1:20">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="1"/>
@@ -4815,7 +5039,7 @@
       <c r="S184" s="1"/>
       <c r="T184" s="1"/>
     </row>
-    <row r="185">
+    <row r="185" spans="1:20">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="1"/>
@@ -4837,7 +5061,7 @@
       <c r="S185" s="1"/>
       <c r="T185" s="1"/>
     </row>
-    <row r="186">
+    <row r="186" spans="1:20">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="1"/>
@@ -4859,7 +5083,7 @@
       <c r="S186" s="1"/>
       <c r="T186" s="1"/>
     </row>
-    <row r="187">
+    <row r="187" spans="1:20">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="1"/>
@@ -4881,7 +5105,7 @@
       <c r="S187" s="1"/>
       <c r="T187" s="1"/>
     </row>
-    <row r="188">
+    <row r="188" spans="1:20">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="1"/>
@@ -4903,7 +5127,7 @@
       <c r="S188" s="1"/>
       <c r="T188" s="1"/>
     </row>
-    <row r="189">
+    <row r="189" spans="1:20">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="1"/>
@@ -4925,7 +5149,7 @@
       <c r="S189" s="1"/>
       <c r="T189" s="1"/>
     </row>
-    <row r="190">
+    <row r="190" spans="1:20">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="1"/>
@@ -4947,7 +5171,7 @@
       <c r="S190" s="1"/>
       <c r="T190" s="1"/>
     </row>
-    <row r="191">
+    <row r="191" spans="1:20">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="1"/>
@@ -4969,7 +5193,7 @@
       <c r="S191" s="1"/>
       <c r="T191" s="1"/>
     </row>
-    <row r="192">
+    <row r="192" spans="1:20">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="1"/>
@@ -4991,7 +5215,7 @@
       <c r="S192" s="1"/>
       <c r="T192" s="1"/>
     </row>
-    <row r="193">
+    <row r="193" spans="1:20">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="1"/>
@@ -5013,7 +5237,7 @@
       <c r="S193" s="1"/>
       <c r="T193" s="1"/>
     </row>
-    <row r="194">
+    <row r="194" spans="1:20">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="1"/>
@@ -5035,7 +5259,7 @@
       <c r="S194" s="1"/>
       <c r="T194" s="1"/>
     </row>
-    <row r="195">
+    <row r="195" spans="1:20">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="1"/>
@@ -5057,7 +5281,7 @@
       <c r="S195" s="1"/>
       <c r="T195" s="1"/>
     </row>
-    <row r="196">
+    <row r="196" spans="1:20">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="1"/>
@@ -5079,7 +5303,7 @@
       <c r="S196" s="1"/>
       <c r="T196" s="1"/>
     </row>
-    <row r="197">
+    <row r="197" spans="1:20">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="1"/>
@@ -5101,7 +5325,7 @@
       <c r="S197" s="1"/>
       <c r="T197" s="1"/>
     </row>
-    <row r="198">
+    <row r="198" spans="1:20">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="1"/>
@@ -5123,7 +5347,7 @@
       <c r="S198" s="1"/>
       <c r="T198" s="1"/>
     </row>
-    <row r="199">
+    <row r="199" spans="1:20">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="1"/>
@@ -5145,7 +5369,7 @@
       <c r="S199" s="1"/>
       <c r="T199" s="1"/>
     </row>
-    <row r="200">
+    <row r="200" spans="1:20">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="1"/>
@@ -5168,6 +5392,7 @@
       <c r="T200" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: ✨I can do it！
</commit_message>
<xml_diff>
--- a/许愿墙.xlsx
+++ b/许愿墙.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\桌面\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3932C32-3F17-47BC-A4A1-2F2E14D69E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="27945" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>你想找什么样的工作？</t>
   </si>
@@ -234,18 +230,22 @@
   </si>
   <si>
     <t>网络安全</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>已经通知面试了</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -268,29 +268,165 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.75"/>
-      <color rgb="FF000000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,8 +439,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -342,9 +664,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -365,24 +929,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -640,28 +1248,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="74" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +1294,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -713,7 +1320,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -739,7 +1346,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -765,7 +1372,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -791,7 +1398,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -817,7 +1424,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -843,7 +1450,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -869,7 +1476,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -895,7 +1502,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -921,7 +1528,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -947,7 +1554,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -973,7 +1580,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -999,7 +1606,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1025,7 +1632,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1051,7 +1658,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -1077,7 +1684,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1710,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -1129,7 +1736,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1155,7 +1762,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1181,7 +1788,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1814,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1233,7 +1840,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1259,7 +1866,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1285,7 +1892,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1918,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1944,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1363,7 +1970,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -1389,7 +1996,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -1415,7 +2022,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1441,7 +2048,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -1467,7 +2074,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32" s="3" t="s">
         <v>25</v>
       </c>
@@ -1493,7 +2100,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20">
       <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
@@ -1519,7 +2126,7 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1545,7 +2152,7 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20">
       <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
@@ -1571,7 +2178,7 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20">
       <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
@@ -1597,7 +2204,7 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20">
       <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +2230,7 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +2256,7 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1675,7 +2282,7 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20">
       <c r="A40" s="3" t="s">
         <v>26</v>
       </c>
@@ -1701,7 +2308,7 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1727,7 +2334,7 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1753,7 +2360,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -1779,7 +2386,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20">
       <c r="A44" s="3" t="s">
         <v>23</v>
       </c>
@@ -1805,7 +2412,7 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
@@ -1831,7 +2438,7 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -1857,7 +2464,7 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -1883,7 +2490,7 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>
@@ -1909,7 +2516,7 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20">
       <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
@@ -1935,7 +2542,7 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20">
       <c r="A50" s="3" t="s">
         <v>51</v>
       </c>
@@ -1961,7 +2568,7 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20">
       <c r="A51" s="3" t="s">
         <v>52</v>
       </c>
@@ -1987,7 +2594,7 @@
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20">
       <c r="A52" s="3" t="s">
         <v>46</v>
       </c>
@@ -2013,7 +2620,7 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
@@ -2039,7 +2646,7 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
@@ -2065,7 +2672,7 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
@@ -2091,7 +2698,7 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20">
       <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
@@ -2117,7 +2724,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
@@ -2143,7 +2750,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2169,7 +2776,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20">
       <c r="A59" s="3" t="s">
         <v>7</v>
       </c>
@@ -2195,7 +2802,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20">
       <c r="A60" s="3" t="s">
         <v>25</v>
       </c>
@@ -2221,7 +2828,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2247,7 +2854,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2273,7 +2880,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20">
       <c r="A63" s="5" t="s">
         <v>62</v>
       </c>
@@ -2299,7 +2906,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2325,7 +2932,7 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20">
       <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
@@ -2351,9 +2958,13 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
+    <row r="66" spans="1:20">
+      <c r="A66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2373,7 +2984,7 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="2"/>
@@ -2395,7 +3006,7 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="2"/>
@@ -2417,7 +3028,7 @@
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="2"/>
@@ -2439,7 +3050,7 @@
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="2"/>
@@ -2461,7 +3072,7 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="2"/>
@@ -2483,7 +3094,7 @@
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="2"/>
@@ -2505,7 +3116,7 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="2"/>
@@ -2527,7 +3138,7 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="2"/>
@@ -2549,7 +3160,7 @@
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="2"/>
@@ -2571,7 +3182,7 @@
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="2"/>
@@ -2593,7 +3204,7 @@
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="2"/>
@@ -2615,7 +3226,7 @@
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="2"/>
@@ -2637,7 +3248,7 @@
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="2"/>
@@ -2659,7 +3270,7 @@
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="2"/>
@@ -2681,7 +3292,7 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="2"/>
@@ -2703,7 +3314,7 @@
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="2"/>
@@ -2725,7 +3336,7 @@
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
@@ -2747,7 +3358,7 @@
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="2"/>
@@ -2769,7 +3380,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="2"/>
@@ -2791,7 +3402,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="2"/>
@@ -2813,7 +3424,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="2"/>
@@ -2835,7 +3446,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="2"/>
@@ -2857,7 +3468,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="2"/>
@@ -2879,7 +3490,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="2"/>
@@ -2901,7 +3512,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="2"/>
@@ -2923,7 +3534,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="2"/>
@@ -2945,7 +3556,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="2"/>
@@ -2967,7 +3578,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="2"/>
@@ -2989,7 +3600,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="2"/>
@@ -3011,7 +3622,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="2"/>
@@ -3033,7 +3644,7 @@
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="2"/>
@@ -3055,7 +3666,7 @@
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="2"/>
@@ -3077,7 +3688,7 @@
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="2"/>
@@ -3099,7 +3710,7 @@
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="2"/>
@@ -3121,7 +3732,7 @@
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="2"/>
@@ -3143,7 +3754,7 @@
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="2"/>
@@ -3165,7 +3776,7 @@
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="2"/>
@@ -3187,7 +3798,7 @@
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="2"/>
@@ -3209,7 +3820,7 @@
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="2"/>
@@ -3231,7 +3842,7 @@
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="2"/>
@@ -3253,7 +3864,7 @@
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="2"/>
@@ -3275,7 +3886,7 @@
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="2"/>
@@ -3297,7 +3908,7 @@
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="2"/>
@@ -3319,7 +3930,7 @@
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="2"/>
@@ -3341,7 +3952,7 @@
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="2"/>
@@ -3363,7 +3974,7 @@
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="2"/>
@@ -3385,7 +3996,7 @@
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="2"/>
@@ -3407,7 +4018,7 @@
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="2"/>
@@ -3429,7 +4040,7 @@
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="2"/>
@@ -3451,7 +4062,7 @@
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="2"/>
@@ -3473,7 +4084,7 @@
       <c r="S116" s="2"/>
       <c r="T116" s="2"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="2"/>
@@ -3495,7 +4106,7 @@
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="2"/>
@@ -3517,7 +4128,7 @@
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="2"/>
@@ -3539,7 +4150,7 @@
       <c r="S119" s="2"/>
       <c r="T119" s="2"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="2"/>
@@ -3561,7 +4172,7 @@
       <c r="S120" s="2"/>
       <c r="T120" s="2"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="2"/>
@@ -3583,7 +4194,7 @@
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="2"/>
@@ -3605,7 +4216,7 @@
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="2"/>
@@ -3627,7 +4238,7 @@
       <c r="S123" s="2"/>
       <c r="T123" s="2"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="2"/>
@@ -3649,7 +4260,7 @@
       <c r="S124" s="2"/>
       <c r="T124" s="2"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="2"/>
@@ -3671,7 +4282,7 @@
       <c r="S125" s="2"/>
       <c r="T125" s="2"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="2"/>
@@ -3693,7 +4304,7 @@
       <c r="S126" s="2"/>
       <c r="T126" s="2"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="2"/>
@@ -3715,7 +4326,7 @@
       <c r="S127" s="2"/>
       <c r="T127" s="2"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="2"/>
@@ -3737,7 +4348,7 @@
       <c r="S128" s="2"/>
       <c r="T128" s="2"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="2"/>
@@ -3759,7 +4370,7 @@
       <c r="S129" s="2"/>
       <c r="T129" s="2"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="2"/>
@@ -3781,7 +4392,7 @@
       <c r="S130" s="2"/>
       <c r="T130" s="2"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="2"/>
@@ -3803,7 +4414,7 @@
       <c r="S131" s="2"/>
       <c r="T131" s="2"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="2"/>
@@ -3825,7 +4436,7 @@
       <c r="S132" s="2"/>
       <c r="T132" s="2"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="2"/>
@@ -3847,7 +4458,7 @@
       <c r="S133" s="2"/>
       <c r="T133" s="2"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="2"/>
@@ -3869,7 +4480,7 @@
       <c r="S134" s="2"/>
       <c r="T134" s="2"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="2"/>
@@ -3891,7 +4502,7 @@
       <c r="S135" s="2"/>
       <c r="T135" s="2"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="2"/>
@@ -3913,7 +4524,7 @@
       <c r="S136" s="2"/>
       <c r="T136" s="2"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="2"/>
@@ -3935,7 +4546,7 @@
       <c r="S137" s="2"/>
       <c r="T137" s="2"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="2"/>
@@ -3957,7 +4568,7 @@
       <c r="S138" s="2"/>
       <c r="T138" s="2"/>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="2"/>
@@ -3979,7 +4590,7 @@
       <c r="S139" s="2"/>
       <c r="T139" s="2"/>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="2"/>
@@ -4001,7 +4612,7 @@
       <c r="S140" s="2"/>
       <c r="T140" s="2"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="2"/>
@@ -4023,7 +4634,7 @@
       <c r="S141" s="2"/>
       <c r="T141" s="2"/>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="2"/>
@@ -4045,7 +4656,7 @@
       <c r="S142" s="2"/>
       <c r="T142" s="2"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="2"/>
@@ -4067,7 +4678,7 @@
       <c r="S143" s="2"/>
       <c r="T143" s="2"/>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="2"/>
@@ -4089,7 +4700,7 @@
       <c r="S144" s="2"/>
       <c r="T144" s="2"/>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="2"/>
@@ -4111,7 +4722,7 @@
       <c r="S145" s="2"/>
       <c r="T145" s="2"/>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="2"/>
@@ -4133,7 +4744,7 @@
       <c r="S146" s="2"/>
       <c r="T146" s="2"/>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="2"/>
@@ -4155,7 +4766,7 @@
       <c r="S147" s="2"/>
       <c r="T147" s="2"/>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="2"/>
@@ -4177,7 +4788,7 @@
       <c r="S148" s="2"/>
       <c r="T148" s="2"/>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="2"/>
@@ -4199,7 +4810,7 @@
       <c r="S149" s="2"/>
       <c r="T149" s="2"/>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="2"/>
@@ -4221,7 +4832,7 @@
       <c r="S150" s="2"/>
       <c r="T150" s="2"/>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="2"/>
@@ -4243,7 +4854,7 @@
       <c r="S151" s="2"/>
       <c r="T151" s="2"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="2"/>
@@ -4265,7 +4876,7 @@
       <c r="S152" s="2"/>
       <c r="T152" s="2"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="2"/>
@@ -4287,7 +4898,7 @@
       <c r="S153" s="2"/>
       <c r="T153" s="2"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="2"/>
@@ -4309,7 +4920,7 @@
       <c r="S154" s="2"/>
       <c r="T154" s="2"/>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="2"/>
@@ -4331,7 +4942,7 @@
       <c r="S155" s="2"/>
       <c r="T155" s="2"/>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="2"/>
@@ -4353,7 +4964,7 @@
       <c r="S156" s="2"/>
       <c r="T156" s="2"/>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="2"/>
@@ -4375,7 +4986,7 @@
       <c r="S157" s="2"/>
       <c r="T157" s="2"/>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="2"/>
@@ -4397,7 +5008,7 @@
       <c r="S158" s="2"/>
       <c r="T158" s="2"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="2"/>
@@ -4419,7 +5030,7 @@
       <c r="S159" s="2"/>
       <c r="T159" s="2"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="2"/>
@@ -4441,7 +5052,7 @@
       <c r="S160" s="2"/>
       <c r="T160" s="2"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="2"/>
@@ -4463,7 +5074,7 @@
       <c r="S161" s="2"/>
       <c r="T161" s="2"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="2"/>
@@ -4485,7 +5096,7 @@
       <c r="S162" s="2"/>
       <c r="T162" s="2"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="2"/>
@@ -4507,7 +5118,7 @@
       <c r="S163" s="2"/>
       <c r="T163" s="2"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="2"/>
@@ -4529,7 +5140,7 @@
       <c r="S164" s="2"/>
       <c r="T164" s="2"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="2"/>
@@ -4551,7 +5162,7 @@
       <c r="S165" s="2"/>
       <c r="T165" s="2"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="2"/>
@@ -4573,7 +5184,7 @@
       <c r="S166" s="2"/>
       <c r="T166" s="2"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="2"/>
@@ -4595,7 +5206,7 @@
       <c r="S167" s="2"/>
       <c r="T167" s="2"/>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="2"/>
@@ -4617,7 +5228,7 @@
       <c r="S168" s="2"/>
       <c r="T168" s="2"/>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="2"/>
@@ -4639,7 +5250,7 @@
       <c r="S169" s="2"/>
       <c r="T169" s="2"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="2"/>
@@ -4661,7 +5272,7 @@
       <c r="S170" s="2"/>
       <c r="T170" s="2"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="2"/>
@@ -4683,7 +5294,7 @@
       <c r="S171" s="2"/>
       <c r="T171" s="2"/>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="2"/>
@@ -4705,7 +5316,7 @@
       <c r="S172" s="2"/>
       <c r="T172" s="2"/>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="2"/>
@@ -4727,7 +5338,7 @@
       <c r="S173" s="2"/>
       <c r="T173" s="2"/>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="2"/>
@@ -4749,7 +5360,7 @@
       <c r="S174" s="2"/>
       <c r="T174" s="2"/>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="2"/>
@@ -4771,7 +5382,7 @@
       <c r="S175" s="2"/>
       <c r="T175" s="2"/>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="2"/>
@@ -4793,7 +5404,7 @@
       <c r="S176" s="2"/>
       <c r="T176" s="2"/>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="2"/>
@@ -4815,7 +5426,7 @@
       <c r="S177" s="2"/>
       <c r="T177" s="2"/>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="2"/>
@@ -4837,7 +5448,7 @@
       <c r="S178" s="2"/>
       <c r="T178" s="2"/>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="2"/>
@@ -4859,7 +5470,7 @@
       <c r="S179" s="2"/>
       <c r="T179" s="2"/>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="2"/>
@@ -4881,7 +5492,7 @@
       <c r="S180" s="2"/>
       <c r="T180" s="2"/>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="2"/>
@@ -4903,7 +5514,7 @@
       <c r="S181" s="2"/>
       <c r="T181" s="2"/>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="2"/>
@@ -4925,7 +5536,7 @@
       <c r="S182" s="2"/>
       <c r="T182" s="2"/>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="2"/>
@@ -4947,7 +5558,7 @@
       <c r="S183" s="2"/>
       <c r="T183" s="2"/>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="2"/>
@@ -4969,7 +5580,7 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="2"/>
@@ -4991,7 +5602,7 @@
       <c r="S185" s="2"/>
       <c r="T185" s="2"/>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="2"/>
@@ -5013,7 +5624,7 @@
       <c r="S186" s="2"/>
       <c r="T186" s="2"/>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="2"/>
@@ -5035,7 +5646,7 @@
       <c r="S187" s="2"/>
       <c r="T187" s="2"/>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="2"/>
@@ -5057,7 +5668,7 @@
       <c r="S188" s="2"/>
       <c r="T188" s="2"/>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="2"/>
@@ -5079,7 +5690,7 @@
       <c r="S189" s="2"/>
       <c r="T189" s="2"/>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="2"/>
@@ -5101,7 +5712,7 @@
       <c r="S190" s="2"/>
       <c r="T190" s="2"/>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="2"/>
@@ -5123,7 +5734,7 @@
       <c r="S191" s="2"/>
       <c r="T191" s="2"/>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="2"/>
@@ -5145,7 +5756,7 @@
       <c r="S192" s="2"/>
       <c r="T192" s="2"/>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="2"/>
@@ -5167,7 +5778,7 @@
       <c r="S193" s="2"/>
       <c r="T193" s="2"/>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="2"/>
@@ -5189,7 +5800,7 @@
       <c r="S194" s="2"/>
       <c r="T194" s="2"/>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="2"/>
@@ -5211,7 +5822,7 @@
       <c r="S195" s="2"/>
       <c r="T195" s="2"/>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="2"/>
@@ -5233,7 +5844,7 @@
       <c r="S196" s="2"/>
       <c r="T196" s="2"/>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="2"/>
@@ -5255,7 +5866,7 @@
       <c r="S197" s="2"/>
       <c r="T197" s="2"/>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="2"/>
@@ -5277,7 +5888,7 @@
       <c r="S198" s="2"/>
       <c r="T198" s="2"/>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="2"/>
@@ -5299,7 +5910,7 @@
       <c r="S199" s="2"/>
       <c r="T199" s="2"/>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="2"/>
@@ -5322,7 +5933,7 @@
       <c r="T200" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>